<commit_message>
Finish study 2 implementation, need 2 pilot
</commit_message>
<xml_diff>
--- a/Assets/ExperimentData/ExperimentQuestions/Question_Archive.xlsx
+++ b/Assets/ExperimentData/ExperimentQuestions/Question_Archive.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20344"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joe\SmallMultiplesWithCharts\smallmultipleswithcharts\Assets\ExperimentData\ExperimentQuestions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Liu\Documents\Joe\SmallMultiplesWithCharts\ImmersiveSM\Assets\ExperimentData\ExperimentQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6780D7B-F5C1-4DE1-85B7-4BB7604838D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BIM" sheetId="1" r:id="rId1"/>
+    <sheet name="BIM" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Bar" sheetId="2" r:id="rId2"/>
+    <sheet name="Bar Study2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="247">
   <si>
     <t>Compare Value (all sensors)</t>
   </si>
@@ -590,12 +592,210 @@
   <si>
     <t>Which year did United States have less food consumption than its Births attended in 1997?</t>
   </si>
+  <si>
+    <t>Trending</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>TaskID</t>
+  </si>
+  <si>
+    <t>TrialID</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>1/31</t>
+  </si>
+  <si>
+    <t>3/33</t>
+  </si>
+  <si>
+    <t>4/34</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>Half-Circle</t>
+  </si>
+  <si>
+    <t>Full-Circle</t>
+  </si>
+  <si>
+    <t>12/30</t>
+  </si>
+  <si>
+    <t>5/23</t>
+  </si>
+  <si>
+    <t>9/15</t>
+  </si>
+  <si>
+    <t>22/28</t>
+  </si>
+  <si>
+    <t>2/20</t>
+  </si>
+  <si>
+    <t>6/24</t>
+  </si>
+  <si>
+    <t>21/27</t>
+  </si>
+  <si>
+    <t>7/25</t>
+  </si>
+  <si>
+    <t>8/14</t>
+  </si>
+  <si>
+    <t>11/29</t>
+  </si>
+  <si>
+    <t>10/16</t>
+  </si>
+  <si>
+    <t>14/32</t>
+  </si>
+  <si>
+    <t>Backup (Manhatan 7/8)</t>
+  </si>
+  <si>
+    <t>Long Distance Fixed Position</t>
+  </si>
+  <si>
+    <t>For sector 4, which country in 2013 had a similar budget as France in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 3, which country in 2013 had a similar budget as France in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 2, which country in 2013 had a similar budget as Australia in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 5, which country in 2013 had a similar budget as Canada in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 4, which country in 2013 had a similar budget as Denmark in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 1, which country in 2013 had a similar budget as Canada in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 2, which country in 2013 had a similar budget as Denmark in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 3, which country in 2013 had a similar budget as Belgium in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 5, which country in 2013 had a similar budget as France in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 3, which country in 2013 had a similar budget as Australia in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 3, which country in 2013 had a similar budget as Denmark in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 5, which country in 2013 had a similar budget as Australia in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 1, which country in 2013 had a similar budget as Denmark in 1983?</t>
+  </si>
+  <si>
+    <t>For sector 3, which country in 1988 had a similar budget as Belgium in 1994?</t>
+  </si>
+  <si>
+    <t>For sector 2, which country in 1980 had a similar budget as Belgium in 2010?</t>
+  </si>
+  <si>
+    <t>For sector 4, which country in 1984 had a similar budget as France in 2002?</t>
+  </si>
+  <si>
+    <t>For sector 2, which country in 2001 had a similar budget as Canada in 2007?</t>
+  </si>
+  <si>
+    <t>For sector 4, which country in 1982 had a similar budget as Denmark in 2012?</t>
+  </si>
+  <si>
+    <t>For sector 5, which country in 1981 had a similar budget as Denmark in 1999?</t>
+  </si>
+  <si>
+    <t>For sector 1, which country in 1991 had a similar budget as France in 2009?</t>
+  </si>
+  <si>
+    <t>For sector 5, which country in 1985 had a similar budget as Canada in 2003?</t>
+  </si>
+  <si>
+    <t>For sector 4, which country in 2000 had a similar budget as Belgium in 2006?</t>
+  </si>
+  <si>
+    <t>For sector 1, which country in 1986 had a similar budget as Canada in 2004?</t>
+  </si>
+  <si>
+    <t>For sector 4, which country in 1987 had a similar budget as Belgium in 1993?</t>
+  </si>
+  <si>
+    <t>For sector 1, which country in 1983 had a similar budget as France in 2013?</t>
+  </si>
+  <si>
+    <t>For sector 5, which country in 1989 had a similar budget as Canada in 1995?</t>
+  </si>
+  <si>
+    <t>For sector 2, which country in 1993 had a similar budget as France in 2011?</t>
+  </si>
+  <si>
+    <t>For sector 3, which country in 1990 had a similar budget as Belgium in 2008?</t>
+  </si>
+  <si>
+    <t>Which year did Belgium have the most budget on sector 4?</t>
+  </si>
+  <si>
+    <t>Which year did Belgium have the most budget on sector 3?</t>
+  </si>
+  <si>
+    <t>Which year did Belgium have the most budget on sector 2?</t>
+  </si>
+  <si>
+    <t>Which year did Canada have the most budget on sector 2?</t>
+  </si>
+  <si>
+    <t>Which year did Canada have the most budget on sector 1?</t>
+  </si>
+  <si>
+    <t>Which year did Canada have the most budget on sector 3?</t>
+  </si>
+  <si>
+    <t>Which year did Denmark have the most budget on sector 3?</t>
+  </si>
+  <si>
+    <t>Which year did Denmark have the most budget on sector 4?</t>
+  </si>
+  <si>
+    <t>Which year did Denmark have the most budget on sector 5?</t>
+  </si>
+  <si>
+    <t>Which year did France have the most budget on sector 3?</t>
+  </si>
+  <si>
+    <t>Barchart</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,8 +846,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -702,8 +924,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -735,11 +969,214 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1005,6 +1442,93 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,36 +1813,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="45.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1796875" style="12" customWidth="1"/>
-    <col min="8" max="8" width="7.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.453125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="45.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1328125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="7.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.1328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1328125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="7.86328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.3984375" style="6" customWidth="1"/>
     <col min="10" max="10" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.54296875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="36.81640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1796875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="39.6328125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="31.6328125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.7265625" style="1"/>
+    <col min="11" max="11" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.59765625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="36.86328125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1328125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="39.59765625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="9.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.59765625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
@@ -1416,7 +1940,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1456,7 +1980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
@@ -1493,7 +2017,7 @@
       </c>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>37</v>
       </c>
@@ -1524,7 +2048,7 @@
       </c>
       <c r="Q5" s="6"/>
     </row>
-    <row r="6" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>27</v>
       </c>
@@ -1551,7 +2075,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
         <v>30</v>
       </c>
@@ -1578,7 +2102,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
     </row>
-    <row r="8" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="57" x14ac:dyDescent="0.45">
       <c r="A8" s="50" t="s">
         <v>143</v>
       </c>
@@ -1607,7 +2131,7 @@
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A9" s="82" t="s">
         <v>151</v>
       </c>
@@ -1631,7 +2155,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="58" t="s">
         <v>145</v>
       </c>
@@ -1657,7 +2181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="62" t="s">
         <v>147</v>
       </c>
@@ -1683,7 +2207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="66" t="s">
         <v>152</v>
       </c>
@@ -1709,7 +2233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" s="70" t="s">
         <v>153</v>
       </c>
@@ -1735,7 +2259,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A14" s="54" t="s">
         <v>146</v>
       </c>
@@ -1761,7 +2285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="84" t="s">
         <v>149</v>
       </c>
@@ -1787,7 +2311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="84" t="s">
         <v>150</v>
       </c>
@@ -1813,7 +2337,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="70" t="s">
         <v>148</v>
       </c>
@@ -1846,45 +2370,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="46.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" style="30" customWidth="1"/>
-    <col min="3" max="4" width="8.7265625" style="30"/>
-    <col min="5" max="5" width="51.6328125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="8.7265625" style="30"/>
-    <col min="9" max="9" width="56.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.59765625" customWidth="1"/>
+    <col min="2" max="2" width="10.73046875" style="30" customWidth="1"/>
+    <col min="3" max="4" width="8.73046875" style="30"/>
+    <col min="5" max="5" width="51.59765625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="8.73046875" style="30"/>
+    <col min="9" max="9" width="56.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.08984375" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.26953125" customWidth="1"/>
-    <col min="14" max="14" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4.6328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="61.453125" customWidth="1"/>
+    <col min="11" max="11" width="6.1328125" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.265625" customWidth="1"/>
+    <col min="14" max="14" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.59765625" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="61.3984375" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.6328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="46.36328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.6328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.59765625" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="46.3984375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.59765625" style="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.59765625" style="20" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="40" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="47.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="47.86328125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="39.3984375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="2" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>161</v>
       </c>
@@ -1953,7 +2477,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="50" t="s">
         <v>166</v>
       </c>
@@ -2037,7 +2561,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="54" t="s">
         <v>167</v>
       </c>
@@ -2123,7 +2647,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="58" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="54" t="s">
         <v>168</v>
       </c>
@@ -2213,7 +2737,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="58" t="s">
         <v>165</v>
       </c>
@@ -2285,7 +2809,7 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="62" t="s">
         <v>169</v>
       </c>
@@ -2357,7 +2881,7 @@
       <c r="AC6" s="1"/>
       <c r="AD6" s="1"/>
     </row>
-    <row r="7" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="62" t="s">
         <v>170</v>
       </c>
@@ -2427,7 +2951,7 @@
       <c r="AC7" s="1"/>
       <c r="AD7" s="1"/>
     </row>
-    <row r="8" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="66" t="s">
         <v>171</v>
       </c>
@@ -2499,7 +3023,7 @@
       <c r="AC8" s="1"/>
       <c r="AD8" s="1"/>
     </row>
-    <row r="9" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="70" t="s">
         <v>172</v>
       </c>
@@ -2571,7 +3095,7 @@
       <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
     </row>
-    <row r="10" spans="1:30" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="70" t="s">
         <v>173</v>
       </c>
@@ -2635,7 +3159,7 @@
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
     </row>
-    <row r="11" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" ht="28.5" x14ac:dyDescent="0.45">
       <c r="I11" s="38" t="s">
         <v>128</v>
       </c>
@@ -2675,7 +3199,7 @@
       <c r="AC11" s="1"/>
       <c r="AD11" s="1"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -2690,7 +3214,7 @@
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -2705,7 +3229,7 @@
       <c r="AC13" s="1"/>
       <c r="AD13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
@@ -2720,7 +3244,7 @@
       <c r="AC14" s="1"/>
       <c r="AD14" s="1"/>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2735,7 +3259,7 @@
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -2750,7 +3274,7 @@
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
     </row>
-    <row r="17" spans="10:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="10:30" x14ac:dyDescent="0.45">
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -2765,7 +3289,7 @@
       <c r="AC17" s="1"/>
       <c r="AD17" s="1"/>
     </row>
-    <row r="18" spans="10:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="10:30" x14ac:dyDescent="0.45">
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2780,7 +3304,7 @@
       <c r="AC18" s="1"/>
       <c r="AD18" s="1"/>
     </row>
-    <row r="19" spans="10:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="10:30" x14ac:dyDescent="0.45">
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -2795,7 +3319,7 @@
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
     </row>
-    <row r="20" spans="10:30" x14ac:dyDescent="0.35">
+    <row r="20" spans="10:30" x14ac:dyDescent="0.45">
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -2810,13 +3334,13 @@
       <c r="AC20" s="1"/>
       <c r="AD20" s="1"/>
     </row>
-    <row r="21" spans="10:30" x14ac:dyDescent="0.35">
+    <row r="21" spans="10:30" x14ac:dyDescent="0.45">
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="10:30" x14ac:dyDescent="0.35">
+    <row r="22" spans="10:30" x14ac:dyDescent="0.45">
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -2826,4 +3350,988 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33F85B2-D947-4B9B-ACF1-57A2930A540B}">
+  <dimension ref="A1:L34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.19921875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.9296875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.6640625" style="117" customWidth="1"/>
+    <col min="6" max="6" width="8.86328125" customWidth="1"/>
+    <col min="7" max="7" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.53125" style="131" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="94" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="121" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="124" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="126"/>
+    </row>
+    <row r="2" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="101" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="98" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="95" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="108" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="116" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="99" t="s">
+        <v>185</v>
+      </c>
+      <c r="H2" s="95" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" s="116" t="s">
+        <v>183</v>
+      </c>
+      <c r="J2" s="129" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="93" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="97">
+        <v>1</v>
+      </c>
+      <c r="C3" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D3" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="115" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="104" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="100">
+        <v>16</v>
+      </c>
+      <c r="H3" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" s="127" t="s">
+        <v>236</v>
+      </c>
+      <c r="J3" s="130">
+        <v>2000</v>
+      </c>
+      <c r="K3" s="128">
+        <v>24</v>
+      </c>
+      <c r="L3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="97">
+        <v>2</v>
+      </c>
+      <c r="C4" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E4" s="115" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="100">
+        <v>17</v>
+      </c>
+      <c r="H4" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" s="127" t="s">
+        <v>240</v>
+      </c>
+      <c r="J4" s="130">
+        <v>2009</v>
+      </c>
+      <c r="K4" s="128">
+        <v>22</v>
+      </c>
+      <c r="L4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B5" s="97">
+        <v>3</v>
+      </c>
+      <c r="C5" s="96">
+        <v>1</v>
+      </c>
+      <c r="D5" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="115" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="100">
+        <v>18</v>
+      </c>
+      <c r="H5" s="96">
+        <v>10</v>
+      </c>
+      <c r="I5" s="127" t="s">
+        <v>242</v>
+      </c>
+      <c r="J5" s="130">
+        <v>2014</v>
+      </c>
+      <c r="K5" s="128">
+        <v>25</v>
+      </c>
+      <c r="L5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="97">
+        <v>4</v>
+      </c>
+      <c r="C6" s="96">
+        <v>2</v>
+      </c>
+      <c r="D6" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="115" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="100">
+        <v>19</v>
+      </c>
+      <c r="H6" s="96">
+        <v>11</v>
+      </c>
+      <c r="I6" s="127" t="s">
+        <v>243</v>
+      </c>
+      <c r="J6" s="130">
+        <v>1988</v>
+      </c>
+      <c r="K6" s="128">
+        <v>34</v>
+      </c>
+      <c r="L6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="97">
+        <v>5</v>
+      </c>
+      <c r="C7" s="96">
+        <v>3</v>
+      </c>
+      <c r="D7" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E7" s="115" t="s">
+        <v>212</v>
+      </c>
+      <c r="F7" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="100">
+        <v>20</v>
+      </c>
+      <c r="H7" s="96">
+        <v>12</v>
+      </c>
+      <c r="I7" s="127" t="s">
+        <v>245</v>
+      </c>
+      <c r="J7" s="130">
+        <v>1995</v>
+      </c>
+      <c r="K7" s="128">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="97">
+        <v>6</v>
+      </c>
+      <c r="C8" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8" s="115" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="100">
+        <v>21</v>
+      </c>
+      <c r="H8" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8" s="127" t="s">
+        <v>237</v>
+      </c>
+      <c r="J8" s="130">
+        <v>2014</v>
+      </c>
+      <c r="K8" s="128">
+        <v>24</v>
+      </c>
+      <c r="L8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9" s="97">
+        <v>7</v>
+      </c>
+      <c r="C9" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D9" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="115" t="s">
+        <v>214</v>
+      </c>
+      <c r="F9" s="104" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="100">
+        <v>22</v>
+      </c>
+      <c r="H9" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="I9" s="127" t="s">
+        <v>239</v>
+      </c>
+      <c r="J9" s="130">
+        <v>2015</v>
+      </c>
+      <c r="K9" s="128">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="97">
+        <v>8</v>
+      </c>
+      <c r="C10" s="96">
+        <v>4</v>
+      </c>
+      <c r="D10" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="115" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="G10" s="100">
+        <v>23</v>
+      </c>
+      <c r="H10" s="96">
+        <v>13</v>
+      </c>
+      <c r="I10" s="127" t="s">
+        <v>243</v>
+      </c>
+      <c r="J10" s="130">
+        <v>1983</v>
+      </c>
+      <c r="K10" s="128">
+        <v>34</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="97">
+        <v>9</v>
+      </c>
+      <c r="C11" s="96">
+        <v>5</v>
+      </c>
+      <c r="D11" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E11" s="115" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="100">
+        <v>24</v>
+      </c>
+      <c r="H11" s="96">
+        <v>14</v>
+      </c>
+      <c r="I11" s="127" t="s">
+        <v>236</v>
+      </c>
+      <c r="J11" s="130">
+        <v>1984</v>
+      </c>
+      <c r="K11" s="128">
+        <v>24</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="97">
+        <v>10</v>
+      </c>
+      <c r="C12" s="96">
+        <v>6</v>
+      </c>
+      <c r="D12" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E12" s="115" t="s">
+        <v>216</v>
+      </c>
+      <c r="F12" s="104" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="100">
+        <v>25</v>
+      </c>
+      <c r="H12" s="96">
+        <v>15</v>
+      </c>
+      <c r="I12" s="127" t="s">
+        <v>244</v>
+      </c>
+      <c r="J12" s="130">
+        <v>2003</v>
+      </c>
+      <c r="K12" s="128">
+        <v>33</v>
+      </c>
+      <c r="L12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="97">
+        <v>11</v>
+      </c>
+      <c r="C13" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E13" s="115" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="100">
+        <v>26</v>
+      </c>
+      <c r="H13" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="I13" s="127" t="s">
+        <v>238</v>
+      </c>
+      <c r="J13" s="130">
+        <v>1992</v>
+      </c>
+      <c r="K13" s="128">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B14" s="97">
+        <v>12</v>
+      </c>
+      <c r="C14" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="115" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="100">
+        <v>27</v>
+      </c>
+      <c r="H14" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14" s="127" t="s">
+        <v>241</v>
+      </c>
+      <c r="J14" s="130">
+        <v>1988</v>
+      </c>
+      <c r="K14" s="128">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B15" s="97">
+        <v>13</v>
+      </c>
+      <c r="C15" s="96">
+        <v>7</v>
+      </c>
+      <c r="D15" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" s="115" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="100">
+        <v>28</v>
+      </c>
+      <c r="H15" s="96">
+        <v>16</v>
+      </c>
+      <c r="I15" s="127" t="s">
+        <v>244</v>
+      </c>
+      <c r="J15" s="130">
+        <v>2010</v>
+      </c>
+      <c r="K15" s="128">
+        <v>33</v>
+      </c>
+      <c r="L15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="97">
+        <v>14</v>
+      </c>
+      <c r="C16" s="96">
+        <v>8</v>
+      </c>
+      <c r="D16" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" s="115" t="s">
+        <v>220</v>
+      </c>
+      <c r="F16" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="100">
+        <v>29</v>
+      </c>
+      <c r="H16" s="96">
+        <v>17</v>
+      </c>
+      <c r="I16" s="127" t="s">
+        <v>245</v>
+      </c>
+      <c r="J16" s="130">
+        <v>1999</v>
+      </c>
+      <c r="K16" s="128">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B17" s="97">
+        <v>15</v>
+      </c>
+      <c r="C17" s="96">
+        <v>9</v>
+      </c>
+      <c r="D17" s="109" t="s">
+        <v>189</v>
+      </c>
+      <c r="E17" s="115" t="s">
+        <v>219</v>
+      </c>
+      <c r="F17" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="110">
+        <v>30</v>
+      </c>
+      <c r="H17" s="105">
+        <v>18</v>
+      </c>
+      <c r="I17" s="127" t="s">
+        <v>236</v>
+      </c>
+      <c r="J17" s="130">
+        <v>2006</v>
+      </c>
+      <c r="K17" s="128">
+        <v>24</v>
+      </c>
+      <c r="L17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A18" s="118" t="s">
+        <v>206</v>
+      </c>
+      <c r="B18" s="119"/>
+      <c r="C18" s="119"/>
+      <c r="D18" s="119"/>
+      <c r="E18" s="119"/>
+      <c r="F18" s="120"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" s="103"/>
+      <c r="B19" s="98" t="s">
+        <v>185</v>
+      </c>
+      <c r="C19" s="95" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="108" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="116" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A20" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="97">
+        <v>1</v>
+      </c>
+      <c r="C20" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" s="111" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="115" t="s">
+        <v>221</v>
+      </c>
+      <c r="F20" s="104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A21" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="97">
+        <v>2</v>
+      </c>
+      <c r="C21" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" s="113" t="s">
+        <v>187</v>
+      </c>
+      <c r="E21" s="115" t="s">
+        <v>222</v>
+      </c>
+      <c r="F21" s="104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A22" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" s="97">
+        <v>3</v>
+      </c>
+      <c r="C22" s="96">
+        <v>1</v>
+      </c>
+      <c r="D22" s="111" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" s="115" t="s">
+        <v>223</v>
+      </c>
+      <c r="F22" s="104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="97">
+        <v>4</v>
+      </c>
+      <c r="C23" s="96">
+        <v>2</v>
+      </c>
+      <c r="D23" s="111" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="115" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="103" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" s="97">
+        <v>5</v>
+      </c>
+      <c r="C24" s="96">
+        <v>3</v>
+      </c>
+      <c r="D24" s="113" t="s">
+        <v>188</v>
+      </c>
+      <c r="E24" s="115" t="s">
+        <v>225</v>
+      </c>
+      <c r="F24" s="104" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A25" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="97">
+        <v>6</v>
+      </c>
+      <c r="C25" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D25" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="115" t="s">
+        <v>226</v>
+      </c>
+      <c r="F25" s="104" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A26" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B26" s="97">
+        <v>7</v>
+      </c>
+      <c r="C26" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="113" t="s">
+        <v>194</v>
+      </c>
+      <c r="E26" s="115" t="s">
+        <v>227</v>
+      </c>
+      <c r="F26" s="104" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A27" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="97">
+        <v>8</v>
+      </c>
+      <c r="C27" s="96">
+        <v>4</v>
+      </c>
+      <c r="D27" s="111" t="s">
+        <v>199</v>
+      </c>
+      <c r="E27" s="115" t="s">
+        <v>228</v>
+      </c>
+      <c r="F27" s="104" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B28" s="97">
+        <v>9</v>
+      </c>
+      <c r="C28" s="96">
+        <v>5</v>
+      </c>
+      <c r="D28" s="111" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" s="115" t="s">
+        <v>229</v>
+      </c>
+      <c r="F28" s="104" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A29" s="103" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29" s="97">
+        <v>10</v>
+      </c>
+      <c r="C29" s="96">
+        <v>6</v>
+      </c>
+      <c r="D29" s="113" t="s">
+        <v>201</v>
+      </c>
+      <c r="E29" s="115" t="s">
+        <v>230</v>
+      </c>
+      <c r="F29" s="104" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A30" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="97">
+        <v>11</v>
+      </c>
+      <c r="C30" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D30" s="112" t="s">
+        <v>202</v>
+      </c>
+      <c r="E30" s="115" t="s">
+        <v>231</v>
+      </c>
+      <c r="F30" s="104" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A31" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B31" s="97">
+        <v>12</v>
+      </c>
+      <c r="C31" s="96" t="s">
+        <v>182</v>
+      </c>
+      <c r="D31" s="113" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" s="115" t="s">
+        <v>232</v>
+      </c>
+      <c r="F31" s="104" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" s="97">
+        <v>13</v>
+      </c>
+      <c r="C32" s="96">
+        <v>7</v>
+      </c>
+      <c r="D32" s="111" t="s">
+        <v>204</v>
+      </c>
+      <c r="E32" s="115" t="s">
+        <v>233</v>
+      </c>
+      <c r="F32" s="104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="97">
+        <v>14</v>
+      </c>
+      <c r="C33" s="96">
+        <v>8</v>
+      </c>
+      <c r="D33" s="111" t="s">
+        <v>205</v>
+      </c>
+      <c r="E33" s="115" t="s">
+        <v>234</v>
+      </c>
+      <c r="F33" s="104" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A34" s="103" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" s="107">
+        <v>15</v>
+      </c>
+      <c r="C34" s="105">
+        <v>9</v>
+      </c>
+      <c r="D34" s="114" t="s">
+        <v>203</v>
+      </c>
+      <c r="E34" s="115" t="s">
+        <v>235</v>
+      </c>
+      <c r="F34" s="106" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D3 D4:D17 D24 D31" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed timelog issue, fixed sceneCounter issue, change text board text a little
</commit_message>
<xml_diff>
--- a/Assets/ExperimentData/ExperimentQuestions/Question_Archive.xlsx
+++ b/Assets/ExperimentData/ExperimentQuestions/Question_Archive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Liu\Documents\Joe\SmallMultiplesWithCharts\ImmersiveSM\Assets\ExperimentData\ExperimentQuestions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6780D7B-F5C1-4DE1-85B7-4BB7604838D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9D3F6D-EBEA-4F2B-9242-F3EC5C5886DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1493,33 +1493,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1529,6 +1502,33 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3356,8 +3356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33F85B2-D947-4B9B-ACF1-57A2930A540B}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3370,24 +3370,24 @@
     <col min="7" max="7" width="6.06640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.19921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="41.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.53125" style="131" customWidth="1"/>
+    <col min="10" max="10" width="9.53125" style="122" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="94" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="126" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="124" t="s">
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="129" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="126"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="131"/>
     </row>
     <row r="2" spans="1:12" s="93" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="101" t="s">
@@ -3417,7 +3417,7 @@
       <c r="I2" s="116" t="s">
         <v>183</v>
       </c>
-      <c r="J2" s="129" t="s">
+      <c r="J2" s="120" t="s">
         <v>2</v>
       </c>
       <c r="K2" s="93" t="s">
@@ -3434,14 +3434,14 @@
       <c r="C3" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="109" t="s">
-        <v>189</v>
+      <c r="D3" s="111" t="s">
+        <v>196</v>
       </c>
       <c r="E3" s="115" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="F3" s="104" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="G3" s="100">
         <v>16</v>
@@ -3449,13 +3449,13 @@
       <c r="H3" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="I3" s="127" t="s">
+      <c r="I3" s="118" t="s">
         <v>236</v>
       </c>
-      <c r="J3" s="130">
+      <c r="J3" s="121">
         <v>2000</v>
       </c>
-      <c r="K3" s="128">
+      <c r="K3" s="119">
         <v>24</v>
       </c>
       <c r="L3">
@@ -3472,14 +3472,14 @@
       <c r="C4" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="109" t="s">
-        <v>189</v>
+      <c r="D4" s="113" t="s">
+        <v>187</v>
       </c>
       <c r="E4" s="115" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="F4" s="104" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="G4" s="100">
         <v>17</v>
@@ -3487,13 +3487,13 @@
       <c r="H4" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="I4" s="127" t="s">
+      <c r="I4" s="118" t="s">
         <v>240</v>
       </c>
-      <c r="J4" s="130">
+      <c r="J4" s="121">
         <v>2009</v>
       </c>
-      <c r="K4" s="128">
+      <c r="K4" s="119">
         <v>22</v>
       </c>
       <c r="L4">
@@ -3510,14 +3510,14 @@
       <c r="C5" s="96">
         <v>1</v>
       </c>
-      <c r="D5" s="109" t="s">
-        <v>189</v>
+      <c r="D5" s="111" t="s">
+        <v>195</v>
       </c>
       <c r="E5" s="115" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F5" s="104" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="G5" s="100">
         <v>18</v>
@@ -3525,13 +3525,13 @@
       <c r="H5" s="96">
         <v>10</v>
       </c>
-      <c r="I5" s="127" t="s">
+      <c r="I5" s="118" t="s">
         <v>242</v>
       </c>
-      <c r="J5" s="130">
+      <c r="J5" s="121">
         <v>2014</v>
       </c>
-      <c r="K5" s="128">
+      <c r="K5" s="119">
         <v>25</v>
       </c>
       <c r="L5">
@@ -3548,11 +3548,11 @@
       <c r="C6" s="96">
         <v>2</v>
       </c>
-      <c r="D6" s="109" t="s">
-        <v>189</v>
+      <c r="D6" s="111" t="s">
+        <v>197</v>
       </c>
       <c r="E6" s="115" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="F6" s="104" t="s">
         <v>90</v>
@@ -3563,13 +3563,13 @@
       <c r="H6" s="96">
         <v>11</v>
       </c>
-      <c r="I6" s="127" t="s">
+      <c r="I6" s="118" t="s">
         <v>243</v>
       </c>
-      <c r="J6" s="130">
+      <c r="J6" s="121">
         <v>1988</v>
       </c>
-      <c r="K6" s="128">
+      <c r="K6" s="119">
         <v>34</v>
       </c>
       <c r="L6">
@@ -3586,14 +3586,14 @@
       <c r="C7" s="96">
         <v>3</v>
       </c>
-      <c r="D7" s="109" t="s">
-        <v>189</v>
+      <c r="D7" s="113" t="s">
+        <v>188</v>
       </c>
       <c r="E7" s="115" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="F7" s="104" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="G7" s="100">
         <v>20</v>
@@ -3601,13 +3601,13 @@
       <c r="H7" s="96">
         <v>12</v>
       </c>
-      <c r="I7" s="127" t="s">
+      <c r="I7" s="118" t="s">
         <v>245</v>
       </c>
-      <c r="J7" s="130">
+      <c r="J7" s="121">
         <v>1995</v>
       </c>
-      <c r="K7" s="128">
+      <c r="K7" s="119">
         <v>20</v>
       </c>
       <c r="L7">
@@ -3624,11 +3624,11 @@
       <c r="C8" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D8" s="109" t="s">
-        <v>189</v>
+      <c r="D8" s="112" t="s">
+        <v>198</v>
       </c>
       <c r="E8" s="115" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="F8" s="104" t="s">
         <v>62</v>
@@ -3639,13 +3639,13 @@
       <c r="H8" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="I8" s="127" t="s">
+      <c r="I8" s="118" t="s">
         <v>237</v>
       </c>
-      <c r="J8" s="130">
+      <c r="J8" s="121">
         <v>2014</v>
       </c>
-      <c r="K8" s="128">
+      <c r="K8" s="119">
         <v>24</v>
       </c>
       <c r="L8">
@@ -3662,11 +3662,11 @@
       <c r="C9" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="109" t="s">
-        <v>189</v>
+      <c r="D9" s="113" t="s">
+        <v>194</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="F9" s="104" t="s">
         <v>67</v>
@@ -3677,13 +3677,13 @@
       <c r="H9" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="I9" s="127" t="s">
+      <c r="I9" s="118" t="s">
         <v>239</v>
       </c>
-      <c r="J9" s="130">
+      <c r="J9" s="121">
         <v>2015</v>
       </c>
-      <c r="K9" s="128">
+      <c r="K9" s="119">
         <v>7</v>
       </c>
       <c r="L9">
@@ -3700,14 +3700,14 @@
       <c r="C10" s="96">
         <v>4</v>
       </c>
-      <c r="D10" s="109" t="s">
-        <v>189</v>
+      <c r="D10" s="111" t="s">
+        <v>199</v>
       </c>
       <c r="E10" s="115" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="F10" s="104" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="G10" s="100">
         <v>23</v>
@@ -3715,13 +3715,13 @@
       <c r="H10" s="96">
         <v>13</v>
       </c>
-      <c r="I10" s="127" t="s">
+      <c r="I10" s="118" t="s">
         <v>243</v>
       </c>
-      <c r="J10" s="130">
+      <c r="J10" s="121">
         <v>1983</v>
       </c>
-      <c r="K10" s="128">
+      <c r="K10" s="119">
         <v>34</v>
       </c>
       <c r="L10">
@@ -3738,14 +3738,14 @@
       <c r="C11" s="96">
         <v>5</v>
       </c>
-      <c r="D11" s="109" t="s">
-        <v>189</v>
+      <c r="D11" s="111" t="s">
+        <v>200</v>
       </c>
       <c r="E11" s="115" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="F11" s="104" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="G11" s="100">
         <v>24</v>
@@ -3753,13 +3753,13 @@
       <c r="H11" s="96">
         <v>14</v>
       </c>
-      <c r="I11" s="127" t="s">
+      <c r="I11" s="118" t="s">
         <v>236</v>
       </c>
-      <c r="J11" s="130">
+      <c r="J11" s="121">
         <v>1984</v>
       </c>
-      <c r="K11" s="128">
+      <c r="K11" s="119">
         <v>24</v>
       </c>
       <c r="L11">
@@ -3776,14 +3776,14 @@
       <c r="C12" s="96">
         <v>6</v>
       </c>
-      <c r="D12" s="109" t="s">
-        <v>189</v>
+      <c r="D12" s="113" t="s">
+        <v>201</v>
       </c>
       <c r="E12" s="115" t="s">
-        <v>216</v>
+        <v>230</v>
       </c>
       <c r="F12" s="104" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="G12" s="100">
         <v>25</v>
@@ -3791,13 +3791,13 @@
       <c r="H12" s="96">
         <v>15</v>
       </c>
-      <c r="I12" s="127" t="s">
+      <c r="I12" s="118" t="s">
         <v>244</v>
       </c>
-      <c r="J12" s="130">
+      <c r="J12" s="121">
         <v>2003</v>
       </c>
-      <c r="K12" s="128">
+      <c r="K12" s="119">
         <v>33</v>
       </c>
       <c r="L12">
@@ -3814,14 +3814,14 @@
       <c r="C13" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D13" s="109" t="s">
-        <v>189</v>
+      <c r="D13" s="112" t="s">
+        <v>202</v>
       </c>
       <c r="E13" s="115" t="s">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="F13" s="104" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G13" s="100">
         <v>26</v>
@@ -3829,13 +3829,13 @@
       <c r="H13" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="I13" s="127" t="s">
+      <c r="I13" s="118" t="s">
         <v>238</v>
       </c>
-      <c r="J13" s="130">
+      <c r="J13" s="121">
         <v>1992</v>
       </c>
-      <c r="K13" s="128">
+      <c r="K13" s="119">
         <v>4</v>
       </c>
       <c r="L13">
@@ -3852,14 +3852,14 @@
       <c r="C14" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D14" s="109" t="s">
+      <c r="D14" s="113" t="s">
         <v>189</v>
       </c>
       <c r="E14" s="115" t="s">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="F14" s="104" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="G14" s="100">
         <v>27</v>
@@ -3867,13 +3867,13 @@
       <c r="H14" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="I14" s="127" t="s">
+      <c r="I14" s="118" t="s">
         <v>241</v>
       </c>
-      <c r="J14" s="130">
+      <c r="J14" s="121">
         <v>1988</v>
       </c>
-      <c r="K14" s="128">
+      <c r="K14" s="119">
         <v>10</v>
       </c>
       <c r="L14">
@@ -3890,14 +3890,14 @@
       <c r="C15" s="96">
         <v>7</v>
       </c>
-      <c r="D15" s="109" t="s">
-        <v>189</v>
+      <c r="D15" s="111" t="s">
+        <v>204</v>
       </c>
       <c r="E15" s="115" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="F15" s="104" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="G15" s="100">
         <v>28</v>
@@ -3905,13 +3905,13 @@
       <c r="H15" s="96">
         <v>16</v>
       </c>
-      <c r="I15" s="127" t="s">
+      <c r="I15" s="118" t="s">
         <v>244</v>
       </c>
-      <c r="J15" s="130">
+      <c r="J15" s="121">
         <v>2010</v>
       </c>
-      <c r="K15" s="128">
+      <c r="K15" s="119">
         <v>33</v>
       </c>
       <c r="L15">
@@ -3928,11 +3928,11 @@
       <c r="C16" s="96">
         <v>8</v>
       </c>
-      <c r="D16" s="109" t="s">
-        <v>189</v>
+      <c r="D16" s="111" t="s">
+        <v>205</v>
       </c>
       <c r="E16" s="115" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
       <c r="F16" s="104" t="s">
         <v>71</v>
@@ -3943,13 +3943,13 @@
       <c r="H16" s="96">
         <v>17</v>
       </c>
-      <c r="I16" s="127" t="s">
+      <c r="I16" s="118" t="s">
         <v>245</v>
       </c>
-      <c r="J16" s="130">
+      <c r="J16" s="121">
         <v>1999</v>
       </c>
-      <c r="K16" s="128">
+      <c r="K16" s="119">
         <v>20</v>
       </c>
       <c r="L16">
@@ -3966,14 +3966,14 @@
       <c r="C17" s="96">
         <v>9</v>
       </c>
-      <c r="D17" s="109" t="s">
-        <v>189</v>
+      <c r="D17" s="114" t="s">
+        <v>203</v>
       </c>
       <c r="E17" s="115" t="s">
-        <v>219</v>
-      </c>
-      <c r="F17" s="104" t="s">
-        <v>92</v>
+        <v>235</v>
+      </c>
+      <c r="F17" s="106" t="s">
+        <v>67</v>
       </c>
       <c r="G17" s="110">
         <v>30</v>
@@ -3981,13 +3981,13 @@
       <c r="H17" s="105">
         <v>18</v>
       </c>
-      <c r="I17" s="127" t="s">
+      <c r="I17" s="118" t="s">
         <v>236</v>
       </c>
-      <c r="J17" s="130">
+      <c r="J17" s="121">
         <v>2006</v>
       </c>
-      <c r="K17" s="128">
+      <c r="K17" s="119">
         <v>24</v>
       </c>
       <c r="L17">
@@ -3995,14 +3995,14 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A18" s="118" t="s">
+      <c r="A18" s="123" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="120"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="125"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A19" s="103"/>
@@ -4032,15 +4032,18 @@
       <c r="C20" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D20" s="111" t="s">
-        <v>196</v>
+      <c r="D20" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E20" s="115" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="F20" s="104" t="s">
-        <v>90</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="H20" s="109"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="104"/>
     </row>
     <row r="21" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A21" s="103" t="s">
@@ -4052,15 +4055,18 @@
       <c r="C21" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="113" t="s">
-        <v>187</v>
+      <c r="D21" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E21" s="115" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="F21" s="104" t="s">
-        <v>90</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H21" s="109"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="104"/>
     </row>
     <row r="22" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="103" t="s">
@@ -4072,15 +4078,18 @@
       <c r="C22" s="96">
         <v>1</v>
       </c>
-      <c r="D22" s="111" t="s">
-        <v>195</v>
+      <c r="D22" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E22" s="115" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="F22" s="104" t="s">
-        <v>90</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H22" s="109"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="104"/>
     </row>
     <row r="23" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" s="103" t="s">
@@ -4092,15 +4101,18 @@
       <c r="C23" s="96">
         <v>2</v>
       </c>
-      <c r="D23" s="111" t="s">
-        <v>197</v>
+      <c r="D23" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E23" s="115" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="F23" s="104" t="s">
         <v>90</v>
       </c>
+      <c r="H23" s="109"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="104"/>
     </row>
     <row r="24" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A24" s="103" t="s">
@@ -4112,15 +4124,18 @@
       <c r="C24" s="96">
         <v>3</v>
       </c>
-      <c r="D24" s="113" t="s">
-        <v>188</v>
+      <c r="D24" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E24" s="115" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="F24" s="104" t="s">
-        <v>71</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H24" s="109"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="104"/>
     </row>
     <row r="25" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="103" t="s">
@@ -4132,15 +4147,18 @@
       <c r="C25" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D25" s="112" t="s">
-        <v>198</v>
+      <c r="D25" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E25" s="115" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="F25" s="104" t="s">
         <v>62</v>
       </c>
+      <c r="H25" s="109"/>
+      <c r="I25" s="115"/>
+      <c r="J25" s="104"/>
     </row>
     <row r="26" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="103" t="s">
@@ -4152,15 +4170,18 @@
       <c r="C26" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D26" s="113" t="s">
-        <v>194</v>
+      <c r="D26" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E26" s="115" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="F26" s="104" t="s">
         <v>67</v>
       </c>
+      <c r="H26" s="109"/>
+      <c r="I26" s="115"/>
+      <c r="J26" s="104"/>
     </row>
     <row r="27" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="103" t="s">
@@ -4172,15 +4193,18 @@
       <c r="C27" s="96">
         <v>4</v>
       </c>
-      <c r="D27" s="111" t="s">
-        <v>199</v>
+      <c r="D27" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E27" s="115" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="F27" s="104" t="s">
-        <v>71</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H27" s="109"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="104"/>
     </row>
     <row r="28" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="103" t="s">
@@ -4192,15 +4216,18 @@
       <c r="C28" s="96">
         <v>5</v>
       </c>
-      <c r="D28" s="111" t="s">
-        <v>200</v>
+      <c r="D28" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E28" s="115" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="F28" s="104" t="s">
-        <v>92</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="H28" s="109"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="104"/>
     </row>
     <row r="29" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" s="103" t="s">
@@ -4212,15 +4239,18 @@
       <c r="C29" s="96">
         <v>6</v>
       </c>
-      <c r="D29" s="113" t="s">
-        <v>201</v>
+      <c r="D29" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E29" s="115" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="F29" s="104" t="s">
-        <v>92</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="H29" s="109"/>
+      <c r="I29" s="115"/>
+      <c r="J29" s="104"/>
     </row>
     <row r="30" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="103" t="s">
@@ -4232,15 +4262,18 @@
       <c r="C30" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D30" s="112" t="s">
-        <v>202</v>
+      <c r="D30" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E30" s="115" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="F30" s="104" t="s">
-        <v>92</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H30" s="109"/>
+      <c r="I30" s="115"/>
+      <c r="J30" s="104"/>
     </row>
     <row r="31" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A31" s="103" t="s">
@@ -4252,15 +4285,18 @@
       <c r="C31" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="113" t="s">
+      <c r="D31" s="109" t="s">
         <v>189</v>
       </c>
       <c r="E31" s="115" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="F31" s="104" t="s">
-        <v>67</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="H31" s="109"/>
+      <c r="I31" s="115"/>
+      <c r="J31" s="104"/>
     </row>
     <row r="32" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A32" s="103" t="s">
@@ -4272,17 +4308,20 @@
       <c r="C32" s="96">
         <v>7</v>
       </c>
-      <c r="D32" s="111" t="s">
-        <v>204</v>
+      <c r="D32" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E32" s="115" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="F32" s="104" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+      <c r="H32" s="109"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="104"/>
+    </row>
+    <row r="33" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" s="103" t="s">
         <v>192</v>
       </c>
@@ -4292,17 +4331,20 @@
       <c r="C33" s="96">
         <v>8</v>
       </c>
-      <c r="D33" s="111" t="s">
-        <v>205</v>
+      <c r="D33" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E33" s="115" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F33" s="104" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H33" s="109"/>
+      <c r="I33" s="115"/>
+      <c r="J33" s="104"/>
+    </row>
+    <row r="34" spans="1:10" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="103" t="s">
         <v>192</v>
       </c>
@@ -4312,15 +4354,18 @@
       <c r="C34" s="105">
         <v>9</v>
       </c>
-      <c r="D34" s="114" t="s">
-        <v>203</v>
+      <c r="D34" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="E34" s="115" t="s">
-        <v>235</v>
-      </c>
-      <c r="F34" s="106" t="s">
-        <v>67</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="F34" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="109"/>
+      <c r="I34" s="115"/>
+      <c r="J34" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4331,7 +4376,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="D3 D4:D17 D24 D31" twoDigitTextYear="1"/>
+    <ignoredError sqref="D7" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>